<commit_message>
feat: stabilize member-consult-measure workflow with korean columns
</commit_message>
<xml_diff>
--- a/data_clean/delivery_flat_2025.xlsx
+++ b/data_clean/delivery_flat_2025.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K573"/>
+  <dimension ref="A1:K592"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -24499,32 +24499,32 @@
     </row>
     <row r="567">
       <c r="A567" s="2" t="n">
-        <v>46002</v>
+        <v>46001</v>
       </c>
       <c r="B567" t="inlineStr">
         <is>
-          <t>김주영</t>
+          <t>한만교</t>
         </is>
       </c>
       <c r="C567" t="inlineStr">
         <is>
-          <t>10082</t>
+          <t>10108</t>
         </is>
       </c>
       <c r="D567" t="inlineStr">
         <is>
-          <t>목</t>
+          <t>수</t>
         </is>
       </c>
       <c r="E567" t="n">
         <v>12</v>
       </c>
       <c r="F567" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G567" t="inlineStr">
         <is>
-          <t>상1,하1</t>
+          <t>셔2</t>
         </is>
       </c>
       <c r="H567" t="inlineStr"/>
@@ -24533,37 +24533,37 @@
         <v>701</v>
       </c>
       <c r="K567" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="568">
       <c r="A568" s="2" t="n">
-        <v>46003</v>
+        <v>46002</v>
       </c>
       <c r="B568" t="inlineStr">
         <is>
-          <t>조규종</t>
+          <t>김주영</t>
         </is>
       </c>
       <c r="C568" t="inlineStr">
         <is>
-          <t>6098</t>
+          <t>10082</t>
         </is>
       </c>
       <c r="D568" t="inlineStr">
         <is>
-          <t>금</t>
+          <t>목</t>
         </is>
       </c>
       <c r="E568" t="n">
         <v>12</v>
       </c>
       <c r="F568" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G568" t="inlineStr">
         <is>
-          <t>상1,하1,셔3</t>
+          <t>상1,하1</t>
         </is>
       </c>
       <c r="H568" t="inlineStr"/>
@@ -24572,76 +24572,76 @@
         <v>701</v>
       </c>
       <c r="K568" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="569">
       <c r="A569" s="2" t="n">
-        <v>46000</v>
+        <v>46003</v>
       </c>
       <c r="B569" t="inlineStr">
         <is>
-          <t>김정대</t>
+          <t>조규종</t>
         </is>
       </c>
       <c r="C569" t="inlineStr">
         <is>
-          <t>10079</t>
+          <t>6098</t>
         </is>
       </c>
       <c r="D569" t="inlineStr">
         <is>
-          <t>화</t>
+          <t>금</t>
         </is>
       </c>
       <c r="E569" t="n">
         <v>12</v>
       </c>
       <c r="F569" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G569" t="inlineStr">
         <is>
-          <t>상1,중1,하2</t>
+          <t>상1,하1,셔3</t>
         </is>
       </c>
       <c r="H569" t="inlineStr"/>
       <c r="I569" t="inlineStr"/>
       <c r="J569" t="n">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K569" t="n">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="570">
       <c r="A570" s="2" t="n">
-        <v>46003</v>
+        <v>46000</v>
       </c>
       <c r="B570" t="inlineStr">
         <is>
-          <t>이주환</t>
+          <t>김정대</t>
         </is>
       </c>
       <c r="C570" t="inlineStr">
         <is>
-          <t>2953</t>
+          <t>10079</t>
         </is>
       </c>
       <c r="D570" t="inlineStr">
         <is>
-          <t>금</t>
+          <t>화</t>
         </is>
       </c>
       <c r="E570" t="n">
         <v>12</v>
       </c>
       <c r="F570" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G570" t="inlineStr">
         <is>
-          <t>상1,중1,하1,셔1</t>
+          <t>상1,중1,하2</t>
         </is>
       </c>
       <c r="H570" t="inlineStr"/>
@@ -24650,124 +24650,869 @@
         <v>702</v>
       </c>
       <c r="K570" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
     </row>
     <row r="571">
       <c r="A571" s="2" t="n">
-        <v>46006</v>
+        <v>46002</v>
       </c>
       <c r="B571" t="inlineStr">
         <is>
-          <t>권재운</t>
+          <t>김영식</t>
         </is>
       </c>
       <c r="C571" t="inlineStr">
         <is>
-          <t>10094</t>
+          <t>9905</t>
         </is>
       </c>
       <c r="D571" t="inlineStr">
         <is>
-          <t>월</t>
+          <t>목</t>
         </is>
       </c>
       <c r="E571" t="n">
         <v>12</v>
       </c>
       <c r="F571" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G571" t="inlineStr">
         <is>
-          <t>상1,하1,셔3</t>
+          <t>상1,하2,셔3</t>
         </is>
       </c>
       <c r="H571" t="inlineStr"/>
       <c r="I571" t="inlineStr"/>
       <c r="J571" t="n">
-        <v>711</v>
+        <v>702</v>
       </c>
       <c r="K571" t="n">
-        <v>5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="572">
       <c r="A572" s="2" t="n">
-        <v>46013</v>
+        <v>46003</v>
       </c>
       <c r="B572" t="inlineStr">
         <is>
-          <t>김민수</t>
+          <t>이주환</t>
         </is>
       </c>
       <c r="C572" t="inlineStr">
         <is>
-          <t>5582</t>
+          <t>2953</t>
         </is>
       </c>
       <c r="D572" t="inlineStr">
         <is>
-          <t>월</t>
+          <t>금</t>
         </is>
       </c>
       <c r="E572" t="n">
         <v>12</v>
       </c>
       <c r="F572" t="n">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="G572" t="inlineStr">
         <is>
-          <t>코트수선</t>
+          <t>상1,중1,하1,셔1</t>
         </is>
       </c>
       <c r="H572" t="inlineStr"/>
       <c r="I572" t="inlineStr"/>
       <c r="J572" t="n">
-        <v>721</v>
+        <v>702</v>
       </c>
       <c r="K572" t="n">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="573">
       <c r="A573" s="2" t="n">
-        <v>46018</v>
+        <v>46000</v>
       </c>
       <c r="B573" t="inlineStr">
         <is>
-          <t>성일용</t>
+          <t>김동수</t>
         </is>
       </c>
       <c r="C573" t="inlineStr">
         <is>
-          <t>3811</t>
+          <t>9491</t>
         </is>
       </c>
       <c r="D573" t="inlineStr">
         <is>
-          <t>토</t>
+          <t>화</t>
         </is>
       </c>
       <c r="E573" t="n">
         <v>12</v>
       </c>
       <c r="F573" t="n">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="G573" t="inlineStr">
         <is>
-          <t>상1,하1,셔1</t>
+          <t>하1 수선</t>
         </is>
       </c>
       <c r="H573" t="inlineStr"/>
       <c r="I573" t="inlineStr"/>
       <c r="J573" t="n">
+        <v>703</v>
+      </c>
+      <c r="K573" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>신덕호</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>7312</t>
+        </is>
+      </c>
+      <c r="D574" t="inlineStr">
+        <is>
+          <t>금</t>
+        </is>
+      </c>
+      <c r="E574" t="n">
+        <v>12</v>
+      </c>
+      <c r="F574" t="n">
+        <v>12</v>
+      </c>
+      <c r="G574" t="inlineStr">
+        <is>
+          <t>코2,하1,셔2</t>
+        </is>
+      </c>
+      <c r="H574" t="inlineStr"/>
+      <c r="I574" t="inlineStr"/>
+      <c r="J574" t="n">
+        <v>703</v>
+      </c>
+      <c r="K574" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" s="2" t="n">
+        <v>46003</v>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>강두현</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>10112</t>
+        </is>
+      </c>
+      <c r="D575" t="inlineStr">
+        <is>
+          <t>금</t>
+        </is>
+      </c>
+      <c r="E575" t="n">
+        <v>12</v>
+      </c>
+      <c r="F575" t="n">
+        <v>12</v>
+      </c>
+      <c r="G575" t="inlineStr">
+        <is>
+          <t>대여복1</t>
+        </is>
+      </c>
+      <c r="H575" t="inlineStr"/>
+      <c r="I575" t="inlineStr"/>
+      <c r="J575" t="n">
+        <v>704</v>
+      </c>
+      <c r="K575" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" s="2" t="n">
+        <v>46006</v>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>권재운</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>10094</t>
+        </is>
+      </c>
+      <c r="D576" t="inlineStr">
+        <is>
+          <t>월</t>
+        </is>
+      </c>
+      <c r="E576" t="n">
+        <v>12</v>
+      </c>
+      <c r="F576" t="n">
+        <v>15</v>
+      </c>
+      <c r="G576" t="inlineStr">
+        <is>
+          <t>상1,하1,셔3</t>
+        </is>
+      </c>
+      <c r="H576" t="inlineStr"/>
+      <c r="I576" t="inlineStr"/>
+      <c r="J576" t="n">
+        <v>711</v>
+      </c>
+      <c r="K576" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" s="2" t="n">
+        <v>46007</v>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>박인영</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>10107</t>
+        </is>
+      </c>
+      <c r="D577" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E577" t="n">
+        <v>12</v>
+      </c>
+      <c r="F577" t="n">
+        <v>16</v>
+      </c>
+      <c r="G577" t="inlineStr">
+        <is>
+          <t>상1,하1,셔2</t>
+        </is>
+      </c>
+      <c r="H577" t="inlineStr"/>
+      <c r="I577" t="inlineStr"/>
+      <c r="J577" t="n">
+        <v>711</v>
+      </c>
+      <c r="K577" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" s="2" t="n">
+        <v>46008</v>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>임요셉</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>5115</t>
+        </is>
+      </c>
+      <c r="D578" t="inlineStr">
+        <is>
+          <t>수</t>
+        </is>
+      </c>
+      <c r="E578" t="n">
+        <v>12</v>
+      </c>
+      <c r="F578" t="n">
+        <v>17</v>
+      </c>
+      <c r="G578" t="inlineStr">
+        <is>
+          <t>셔2</t>
+        </is>
+      </c>
+      <c r="H578" t="inlineStr"/>
+      <c r="I578" t="inlineStr">
+        <is>
+          <t>택배</t>
+        </is>
+      </c>
+      <c r="J578" t="n">
+        <v>711</v>
+      </c>
+      <c r="K578" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" s="2" t="n">
+        <v>46013</v>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>김민수</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>5582</t>
+        </is>
+      </c>
+      <c r="D579" t="inlineStr">
+        <is>
+          <t>월</t>
+        </is>
+      </c>
+      <c r="E579" t="n">
+        <v>12</v>
+      </c>
+      <c r="F579" t="n">
+        <v>22</v>
+      </c>
+      <c r="G579" t="inlineStr">
+        <is>
+          <t>코트수선</t>
+        </is>
+      </c>
+      <c r="H579" t="inlineStr"/>
+      <c r="I579" t="inlineStr"/>
+      <c r="J579" t="n">
         <v>721</v>
       </c>
-      <c r="K573" t="n">
+      <c r="K579" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>김유현</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>7464</t>
+        </is>
+      </c>
+      <c r="D580" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E580" t="n">
+        <v>12</v>
+      </c>
+      <c r="F580" t="n">
+        <v>23</v>
+      </c>
+      <c r="G580" t="inlineStr">
+        <is>
+          <t>상1,하2,셔2</t>
+        </is>
+      </c>
+      <c r="H580" t="inlineStr"/>
+      <c r="I580" t="inlineStr"/>
+      <c r="J580" t="n">
+        <v>721</v>
+      </c>
+      <c r="K580" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" s="2" t="n">
+        <v>46018</v>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>성일용</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>3811</t>
+        </is>
+      </c>
+      <c r="D581" t="inlineStr">
+        <is>
+          <t>토</t>
+        </is>
+      </c>
+      <c r="E581" t="n">
+        <v>12</v>
+      </c>
+      <c r="F581" t="n">
+        <v>27</v>
+      </c>
+      <c r="G581" t="inlineStr">
+        <is>
+          <t>상1,하1,셔1</t>
+        </is>
+      </c>
+      <c r="H581" t="inlineStr"/>
+      <c r="I581" t="inlineStr"/>
+      <c r="J581" t="n">
+        <v>721</v>
+      </c>
+      <c r="K581" t="n">
         <v>25</v>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" s="2" t="n">
+        <v>46013</v>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>장창석</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>10109</t>
+        </is>
+      </c>
+      <c r="D582" t="inlineStr">
+        <is>
+          <t>월</t>
+        </is>
+      </c>
+      <c r="E582" t="n">
+        <v>12</v>
+      </c>
+      <c r="F582" t="n">
+        <v>22</v>
+      </c>
+      <c r="G582" t="inlineStr">
+        <is>
+          <t>상1,하1,셔2</t>
+        </is>
+      </c>
+      <c r="H582" t="inlineStr"/>
+      <c r="I582" t="inlineStr"/>
+      <c r="J582" t="n">
+        <v>722</v>
+      </c>
+      <c r="K582" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>이세한</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>7399</t>
+        </is>
+      </c>
+      <c r="D583" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E583" t="n">
+        <v>12</v>
+      </c>
+      <c r="F583" t="n">
+        <v>23</v>
+      </c>
+      <c r="G583" t="inlineStr">
+        <is>
+          <t>상1,하1,셔2</t>
+        </is>
+      </c>
+      <c r="H583" t="inlineStr"/>
+      <c r="I583" t="inlineStr"/>
+      <c r="J583" t="n">
+        <v>722</v>
+      </c>
+      <c r="K583" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" s="2" t="n">
+        <v>46013</v>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>염기태</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>10110</t>
+        </is>
+      </c>
+      <c r="D584" t="inlineStr">
+        <is>
+          <t>월</t>
+        </is>
+      </c>
+      <c r="E584" t="n">
+        <v>12</v>
+      </c>
+      <c r="F584" t="n">
+        <v>22</v>
+      </c>
+      <c r="G584" t="inlineStr">
+        <is>
+          <t>상1,하2,셔2</t>
+        </is>
+      </c>
+      <c r="H584" t="inlineStr"/>
+      <c r="I584" t="inlineStr"/>
+      <c r="J584" t="n">
+        <v>723</v>
+      </c>
+      <c r="K584" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>배주원</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>10105</t>
+        </is>
+      </c>
+      <c r="D585" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E585" t="n">
+        <v>12</v>
+      </c>
+      <c r="F585" t="n">
+        <v>23</v>
+      </c>
+      <c r="G585" t="inlineStr">
+        <is>
+          <t>상2,하2,셔3</t>
+        </is>
+      </c>
+      <c r="H585" t="inlineStr"/>
+      <c r="I585" t="inlineStr"/>
+      <c r="J585" t="n">
+        <v>723</v>
+      </c>
+      <c r="K585" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>이현철</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>10102</t>
+        </is>
+      </c>
+      <c r="D586" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E586" t="n">
+        <v>12</v>
+      </c>
+      <c r="F586" t="n">
+        <v>23</v>
+      </c>
+      <c r="G586" t="inlineStr">
+        <is>
+          <t>상1,하1,셔1</t>
+        </is>
+      </c>
+      <c r="H586" t="inlineStr"/>
+      <c r="I586" t="inlineStr"/>
+      <c r="J586" t="n">
+        <v>724</v>
+      </c>
+      <c r="K586" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>이상윤</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>10114</t>
+        </is>
+      </c>
+      <c r="D587" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E587" t="n">
+        <v>12</v>
+      </c>
+      <c r="F587" t="n">
+        <v>23</v>
+      </c>
+      <c r="G587" t="inlineStr">
+        <is>
+          <t>코1,상1,하1,셔1</t>
+        </is>
+      </c>
+      <c r="H587" t="inlineStr"/>
+      <c r="I587" t="inlineStr"/>
+      <c r="J587" t="n">
+        <v>725</v>
+      </c>
+      <c r="K587" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>김재현</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>6053</t>
+        </is>
+      </c>
+      <c r="D588" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E588" t="n">
+        <v>12</v>
+      </c>
+      <c r="F588" t="n">
+        <v>23</v>
+      </c>
+      <c r="G588" t="inlineStr">
+        <is>
+          <t>코1</t>
+        </is>
+      </c>
+      <c r="H588" t="inlineStr"/>
+      <c r="I588" t="inlineStr"/>
+      <c r="J588" t="n">
+        <v>726</v>
+      </c>
+      <c r="K588" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" s="2" t="n">
+        <v>46014</v>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>김준후</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>9923</t>
+        </is>
+      </c>
+      <c r="D589" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E589" t="n">
+        <v>12</v>
+      </c>
+      <c r="F589" t="n">
+        <v>23</v>
+      </c>
+      <c r="G589" t="inlineStr">
+        <is>
+          <t>상1,하1,셔2</t>
+        </is>
+      </c>
+      <c r="H589" t="inlineStr"/>
+      <c r="I589" t="inlineStr"/>
+      <c r="J589" t="n">
+        <v>727</v>
+      </c>
+      <c r="K589" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" s="2" t="n">
+        <v>46020</v>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>이용정</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>10111</t>
+        </is>
+      </c>
+      <c r="D590" t="inlineStr">
+        <is>
+          <t>월</t>
+        </is>
+      </c>
+      <c r="E590" t="n">
+        <v>12</v>
+      </c>
+      <c r="F590" t="n">
+        <v>29</v>
+      </c>
+      <c r="G590" t="inlineStr">
+        <is>
+          <t>대여복2</t>
+        </is>
+      </c>
+      <c r="H590" t="inlineStr"/>
+      <c r="I590" t="inlineStr"/>
+      <c r="J590" t="n">
+        <v>731</v>
+      </c>
+      <c r="K590" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" s="2" t="n">
+        <v>46021</v>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>박정환</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>10113</t>
+        </is>
+      </c>
+      <c r="D591" t="inlineStr">
+        <is>
+          <t>화</t>
+        </is>
+      </c>
+      <c r="E591" t="n">
+        <v>12</v>
+      </c>
+      <c r="F591" t="n">
+        <v>30</v>
+      </c>
+      <c r="G591" t="inlineStr">
+        <is>
+          <t>코1,셔1</t>
+        </is>
+      </c>
+      <c r="H591" t="inlineStr"/>
+      <c r="I591" t="inlineStr"/>
+      <c r="J591" t="n">
+        <v>731</v>
+      </c>
+      <c r="K591" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" s="2" t="n">
+        <v>46020</v>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>박상언</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>10106</t>
+        </is>
+      </c>
+      <c r="D592" t="inlineStr">
+        <is>
+          <t>월</t>
+        </is>
+      </c>
+      <c r="E592" t="n">
+        <v>12</v>
+      </c>
+      <c r="F592" t="n">
+        <v>29</v>
+      </c>
+      <c r="G592" t="inlineStr">
+        <is>
+          <t>상1,하2,셔2</t>
+        </is>
+      </c>
+      <c r="H592" t="inlineStr"/>
+      <c r="I592" t="inlineStr"/>
+      <c r="J592" t="n">
+        <v>732</v>
+      </c>
+      <c r="K592" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>